<commit_message>
Added compnay RNAseq results and modified STAR alignment parameters
</commit_message>
<xml_diff>
--- a/bioinformatics/Logs/RNAseq-alignment-stats.xlsx
+++ b/bioinformatics/Logs/RNAseq-alignment-stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bryce\Documents\scutellariaMetabolites\bioinformatics\Logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05EEFF4C-EE6D-4AC9-AB25-DA28CFEAEEE6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4D9D758-1C88-43C6-B76B-89262BE88E2C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{6382A5D9-1C64-42BE-963F-68A5DFDB5DBD}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Parameters set: --outFilterMismatchNmax 2</t>
   </si>
@@ -99,6 +99,9 @@
   </si>
   <si>
     <t>Summary of STAR alignment of baicalensis (SRP179837) and racemosa (RAC) RNAseq data to baicalensis reference genome</t>
+  </si>
+  <si>
+    <t>Average insert length</t>
   </si>
 </sst>
 </file>
@@ -452,10 +455,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AEAA5B5-83E9-4E99-A6EF-220A13F54802}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -467,20 +470,21 @@
     <col min="5" max="5" width="22.85546875" customWidth="1"/>
     <col min="6" max="6" width="29" customWidth="1"/>
     <col min="7" max="7" width="29.28515625" customWidth="1"/>
-    <col min="8" max="8" width="24.28515625" customWidth="1"/>
+    <col min="8" max="8" width="29.7109375" customWidth="1"/>
+    <col min="9" max="9" width="27.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -494,19 +498,22 @@
         <v>4</v>
       </c>
       <c r="E3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" t="s">
         <v>5</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>6</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>7</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -519,20 +526,23 @@
       <c r="D4" s="1">
         <v>0.61260000000000003</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4">
+        <v>2.1</v>
+      </c>
+      <c r="F4" s="1">
         <v>0.1062</v>
       </c>
-      <c r="F4" s="2">
-        <v>0</v>
-      </c>
-      <c r="G4" s="1">
+      <c r="G4" s="2">
+        <v>0</v>
+      </c>
+      <c r="H4" s="1">
         <v>0.27910000000000001</v>
       </c>
-      <c r="H4" s="1">
+      <c r="I4" s="1">
         <v>4.0000000000000002E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -545,20 +555,23 @@
       <c r="D5" s="1">
         <v>0.6079</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5">
+        <v>2.17</v>
+      </c>
+      <c r="F5" s="1">
         <v>9.7000000000000003E-2</v>
       </c>
-      <c r="F5" s="2">
-        <v>0</v>
-      </c>
-      <c r="G5" s="1">
+      <c r="G5" s="2">
+        <v>0</v>
+      </c>
+      <c r="H5" s="1">
         <v>0.2928</v>
       </c>
-      <c r="H5" s="1">
+      <c r="I5" s="1">
         <v>5.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -571,20 +584,23 @@
       <c r="D6" s="1">
         <v>0.55930000000000002</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6">
+        <v>2.1</v>
+      </c>
+      <c r="F6" s="1">
         <v>8.0799999999999997E-2</v>
       </c>
-      <c r="F6" s="2">
-        <v>0</v>
-      </c>
-      <c r="G6" s="1">
+      <c r="G6" s="2">
+        <v>0</v>
+      </c>
+      <c r="H6" s="1">
         <v>0.3589</v>
       </c>
-      <c r="H6" s="1">
+      <c r="I6" s="1">
         <v>4.0000000000000002E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -597,20 +613,23 @@
       <c r="D7" s="1">
         <v>0.58979999999999999</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7">
+        <v>2.11</v>
+      </c>
+      <c r="F7" s="1">
         <v>0.1111</v>
       </c>
-      <c r="F7" s="2">
-        <v>0</v>
-      </c>
-      <c r="G7" s="1">
+      <c r="G7" s="2">
+        <v>0</v>
+      </c>
+      <c r="H7" s="1">
         <v>0.29799999999999999</v>
       </c>
-      <c r="H7" s="1">
+      <c r="I7" s="1">
         <v>5.9999999999999995E-4</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -623,20 +642,23 @@
       <c r="D8" s="1">
         <v>0.60709999999999997</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8">
+        <v>2.25</v>
+      </c>
+      <c r="F8" s="1">
         <v>9.7600000000000006E-2</v>
       </c>
-      <c r="F8" s="2">
-        <v>0</v>
-      </c>
-      <c r="G8" s="1">
+      <c r="G8" s="2">
+        <v>0</v>
+      </c>
+      <c r="H8" s="1">
         <v>0.29420000000000002</v>
       </c>
-      <c r="H8" s="1">
+      <c r="I8" s="1">
         <v>5.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -649,20 +671,23 @@
       <c r="D9" s="1">
         <v>0.63580000000000003</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9">
+        <v>2.14</v>
+      </c>
+      <c r="F9" s="1">
         <v>0.1022</v>
       </c>
-      <c r="F9" s="2">
-        <v>0</v>
-      </c>
-      <c r="G9" s="1">
+      <c r="G9" s="2">
+        <v>0</v>
+      </c>
+      <c r="H9" s="1">
         <v>0.26100000000000001</v>
       </c>
-      <c r="H9" s="1">
+      <c r="I9" s="1">
         <v>2.9999999999999997E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -675,20 +700,23 @@
       <c r="D10" s="1">
         <v>9.0399999999999994E-2</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10">
+        <v>2.09</v>
+      </c>
+      <c r="F10" s="1">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="F10" s="2">
-        <v>0</v>
-      </c>
-      <c r="G10" s="1">
+      <c r="G10" s="2">
+        <v>0</v>
+      </c>
+      <c r="H10" s="1">
         <v>0.89149999999999996</v>
       </c>
-      <c r="H10" s="1">
+      <c r="I10" s="1">
         <v>1E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -701,20 +729,23 @@
       <c r="D11" s="1">
         <v>8.7400000000000005E-2</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11">
+        <v>2.02</v>
+      </c>
+      <c r="F11" s="1">
         <v>1.9199999999999998E-2</v>
       </c>
-      <c r="F11" s="2">
-        <v>0</v>
-      </c>
-      <c r="G11" s="1">
+      <c r="G11" s="2">
+        <v>0</v>
+      </c>
+      <c r="H11" s="1">
         <v>0.89319999999999999</v>
       </c>
-      <c r="H11" s="1">
+      <c r="I11" s="1">
         <v>1E-4</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -727,20 +758,23 @@
       <c r="D12" s="1">
         <v>9.8299999999999998E-2</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12">
+        <v>2.08</v>
+      </c>
+      <c r="F12" s="1">
         <v>1.9599999999999999E-2</v>
       </c>
-      <c r="F12" s="2">
-        <v>0</v>
-      </c>
-      <c r="G12" s="1">
+      <c r="G12" s="2">
+        <v>0</v>
+      </c>
+      <c r="H12" s="1">
         <v>0.88190000000000002</v>
       </c>
-      <c r="H12" s="1">
+      <c r="I12" s="1">
         <v>1E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -753,20 +787,23 @@
       <c r="D13" s="1">
         <v>8.4000000000000005E-2</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E13">
+        <v>2.06</v>
+      </c>
+      <c r="F13" s="1">
         <v>1.8499999999999999E-2</v>
       </c>
-      <c r="F13" s="2">
-        <v>0</v>
-      </c>
-      <c r="G13" s="1">
+      <c r="G13" s="2">
+        <v>0</v>
+      </c>
+      <c r="H13" s="1">
         <v>0.89729999999999999</v>
       </c>
-      <c r="H13" s="1">
+      <c r="I13" s="1">
         <v>2.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -779,20 +816,23 @@
       <c r="D14" s="1">
         <v>9.5500000000000002E-2</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E14">
+        <v>2.13</v>
+      </c>
+      <c r="F14" s="1">
         <v>2.24E-2</v>
       </c>
-      <c r="F14" s="2">
-        <v>0</v>
-      </c>
-      <c r="G14" s="1">
+      <c r="G14" s="2">
+        <v>0</v>
+      </c>
+      <c r="H14" s="1">
         <v>0.88180000000000003</v>
       </c>
-      <c r="H14" s="1">
+      <c r="I14" s="1">
         <v>2.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -805,16 +845,19 @@
       <c r="D15" s="1">
         <v>0.1016</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E15">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F15" s="1">
         <v>2.41E-2</v>
       </c>
-      <c r="F15" s="2">
-        <v>0</v>
-      </c>
-      <c r="G15" s="1">
+      <c r="G15" s="2">
+        <v>0</v>
+      </c>
+      <c r="H15" s="1">
         <v>0.87409999999999999</v>
       </c>
-      <c r="H15" s="1">
+      <c r="I15" s="1">
         <v>2.0000000000000001E-4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added stats for novoalign and STAR rerun
</commit_message>
<xml_diff>
--- a/bioinformatics/Logs/RNAseq-alignment-stats.xlsx
+++ b/bioinformatics/Logs/RNAseq-alignment-stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bryce\Documents\scutellariaMetabolites\bioinformatics\Logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4D9D758-1C88-43C6-B76B-89262BE88E2C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BADB6E64-46AB-434B-B59C-1C02CA8E235A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{6382A5D9-1C64-42BE-963F-68A5DFDB5DBD}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="24">
   <si>
     <t>Parameters set: --outFilterMismatchNmax 2</t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t>Average insert length</t>
+  </si>
+  <si>
+    <t>Parameters set: --outFilterScoreMinOverLread 0 --outFilterMatchNminOverLread 0 --outFilterMatchNmin 0 --outFilterMismatchNmax 2</t>
   </si>
 </sst>
 </file>
@@ -455,10 +458,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AEAA5B5-83E9-4E99-A6EF-220A13F54802}">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -861,6 +864,388 @@
         <v>2.0000000000000001E-4</v>
       </c>
     </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" t="s">
+        <v>4</v>
+      </c>
+      <c r="E18" t="s">
+        <v>22</v>
+      </c>
+      <c r="F18" t="s">
+        <v>5</v>
+      </c>
+      <c r="G18" t="s">
+        <v>6</v>
+      </c>
+      <c r="H18" t="s">
+        <v>7</v>
+      </c>
+      <c r="I18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19">
+        <v>22595120</v>
+      </c>
+      <c r="C19">
+        <v>300</v>
+      </c>
+      <c r="D19" s="1">
+        <v>0.79969999999999997</v>
+      </c>
+      <c r="E19">
+        <v>2.27</v>
+      </c>
+      <c r="F19" s="1">
+        <v>0.1973</v>
+      </c>
+      <c r="G19" s="2">
+        <v>0</v>
+      </c>
+      <c r="H19" s="2">
+        <v>0</v>
+      </c>
+      <c r="I19" s="1">
+        <v>4.0000000000000002E-4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20">
+        <v>25589730</v>
+      </c>
+      <c r="C20">
+        <v>300</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0.80400000000000005</v>
+      </c>
+      <c r="E20">
+        <v>2.44</v>
+      </c>
+      <c r="F20" s="1">
+        <v>0.19259999999999999</v>
+      </c>
+      <c r="G20" s="2">
+        <v>0</v>
+      </c>
+      <c r="H20" s="2">
+        <v>0</v>
+      </c>
+      <c r="I20" s="1">
+        <v>5.0000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21">
+        <v>48528038</v>
+      </c>
+      <c r="C21">
+        <v>300</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0.7268</v>
+      </c>
+      <c r="E21">
+        <v>2.27</v>
+      </c>
+      <c r="F21" s="1">
+        <v>0.26469999999999999</v>
+      </c>
+      <c r="G21" s="2">
+        <v>0</v>
+      </c>
+      <c r="H21" s="2">
+        <v>0</v>
+      </c>
+      <c r="I21" s="1">
+        <v>4.0000000000000002E-4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22">
+        <v>41235603</v>
+      </c>
+      <c r="C22">
+        <v>300</v>
+      </c>
+      <c r="D22" s="1">
+        <v>0.76500000000000001</v>
+      </c>
+      <c r="E22">
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="F22" s="1">
+        <v>0.23150000000000001</v>
+      </c>
+      <c r="G22" s="2">
+        <v>0</v>
+      </c>
+      <c r="H22" s="2">
+        <v>0</v>
+      </c>
+      <c r="I22" s="1">
+        <v>5.9999999999999995E-4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23">
+        <v>20852584</v>
+      </c>
+      <c r="C23">
+        <v>300</v>
+      </c>
+      <c r="D23" s="1">
+        <v>0.78710000000000002</v>
+      </c>
+      <c r="E23">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="F23" s="1">
+        <v>0.2094</v>
+      </c>
+      <c r="G23" s="2">
+        <v>0</v>
+      </c>
+      <c r="H23" s="2">
+        <v>0</v>
+      </c>
+      <c r="I23" s="1">
+        <v>5.0000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24">
+        <v>18571158</v>
+      </c>
+      <c r="C24">
+        <v>300</v>
+      </c>
+      <c r="D24" s="1">
+        <v>0.79220000000000002</v>
+      </c>
+      <c r="E24">
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="F24" s="1">
+        <v>0.20449999999999999</v>
+      </c>
+      <c r="G24" s="2">
+        <v>0</v>
+      </c>
+      <c r="H24" s="2">
+        <v>0</v>
+      </c>
+      <c r="I24" s="1">
+        <v>2.9999999999999997E-4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>15</v>
+      </c>
+      <c r="B25">
+        <v>38680165</v>
+      </c>
+      <c r="C25">
+        <v>202</v>
+      </c>
+      <c r="D25" s="1">
+        <v>0.69489999999999996</v>
+      </c>
+      <c r="E25">
+        <v>2.76</v>
+      </c>
+      <c r="F25" s="1">
+        <v>0.29849999999999999</v>
+      </c>
+      <c r="G25" s="2">
+        <v>0</v>
+      </c>
+      <c r="H25" s="2">
+        <v>0</v>
+      </c>
+      <c r="I25" s="1">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>16</v>
+      </c>
+      <c r="B26">
+        <v>39743330</v>
+      </c>
+      <c r="C26">
+        <v>202</v>
+      </c>
+      <c r="D26" s="1">
+        <v>0.69</v>
+      </c>
+      <c r="E26">
+        <v>2.69</v>
+      </c>
+      <c r="F26" s="1">
+        <v>0.30309999999999998</v>
+      </c>
+      <c r="G26" s="2">
+        <v>0</v>
+      </c>
+      <c r="H26" s="2">
+        <v>0</v>
+      </c>
+      <c r="I26" s="1">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>17</v>
+      </c>
+      <c r="B27">
+        <v>31208809</v>
+      </c>
+      <c r="C27">
+        <v>202</v>
+      </c>
+      <c r="D27" s="1">
+        <v>0.71150000000000002</v>
+      </c>
+      <c r="E27">
+        <v>2.6</v>
+      </c>
+      <c r="F27" s="1">
+        <v>0.28270000000000001</v>
+      </c>
+      <c r="G27" s="2">
+        <v>0</v>
+      </c>
+      <c r="H27" s="2">
+        <v>0</v>
+      </c>
+      <c r="I27" s="1">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28">
+        <v>32802143</v>
+      </c>
+      <c r="C28">
+        <v>202</v>
+      </c>
+      <c r="D28" s="1">
+        <v>0.70830000000000004</v>
+      </c>
+      <c r="E28">
+        <v>2.5299999999999998</v>
+      </c>
+      <c r="F28" s="1">
+        <v>0.28549999999999998</v>
+      </c>
+      <c r="G28" s="2">
+        <v>0</v>
+      </c>
+      <c r="H28" s="2">
+        <v>0</v>
+      </c>
+      <c r="I28" s="1">
+        <v>2.0000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>18</v>
+      </c>
+      <c r="B29">
+        <v>29613922</v>
+      </c>
+      <c r="C29">
+        <v>202</v>
+      </c>
+      <c r="D29" s="1">
+        <v>0.73199999999999998</v>
+      </c>
+      <c r="E29">
+        <v>2.61</v>
+      </c>
+      <c r="F29" s="1">
+        <v>0.2641</v>
+      </c>
+      <c r="G29" s="2">
+        <v>0</v>
+      </c>
+      <c r="H29" s="2">
+        <v>0</v>
+      </c>
+      <c r="I29" s="1">
+        <v>2.0000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>19</v>
+      </c>
+      <c r="B30">
+        <v>35774916</v>
+      </c>
+      <c r="C30">
+        <v>202</v>
+      </c>
+      <c r="D30" s="1">
+        <v>0.73040000000000005</v>
+      </c>
+      <c r="E30">
+        <v>2.67</v>
+      </c>
+      <c r="F30" s="1">
+        <v>0.2651</v>
+      </c>
+      <c r="G30" s="2">
+        <v>0</v>
+      </c>
+      <c r="H30" s="2">
+        <v>0</v>
+      </c>
+      <c r="I30" s="1">
+        <v>2.0000000000000001E-4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added logs for v3 STAR alignment
</commit_message>
<xml_diff>
--- a/bioinformatics/Logs/RNAseq-alignment-stats.xlsx
+++ b/bioinformatics/Logs/RNAseq-alignment-stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bryce\Documents\scutellariaMetabolites\bioinformatics\Logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BADB6E64-46AB-434B-B59C-1C02CA8E235A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B76D6F2-94B4-4BDF-8CF9-57A1095042F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{6382A5D9-1C64-42BE-963F-68A5DFDB5DBD}"/>
+    <workbookView xWindow="20400" yWindow="10515" windowWidth="19005" windowHeight="15600" xr2:uid="{6382A5D9-1C64-42BE-963F-68A5DFDB5DBD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="26">
   <si>
     <t>Parameters set: --outFilterMismatchNmax 2</t>
   </si>
@@ -105,6 +105,12 @@
   </si>
   <si>
     <t>Parameters set: --outFilterScoreMinOverLread 0 --outFilterMatchNminOverLread 0 --outFilterMatchNmin 0 --outFilterMismatchNmax 2</t>
+  </si>
+  <si>
+    <t>With trimmomatic first applied to remove adapter sequences</t>
+  </si>
+  <si>
+    <t>Parameters set: none</t>
   </si>
 </sst>
 </file>
@@ -140,10 +146,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -458,10 +466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AEAA5B5-83E9-4E99-A6EF-220A13F54802}">
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="D19" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1246,6 +1254,393 @@
         <v>2.0000000000000001E-4</v>
       </c>
     </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>1</v>
+      </c>
+      <c r="B34" t="s">
+        <v>2</v>
+      </c>
+      <c r="C34" t="s">
+        <v>3</v>
+      </c>
+      <c r="D34" t="s">
+        <v>4</v>
+      </c>
+      <c r="E34" t="s">
+        <v>22</v>
+      </c>
+      <c r="F34" t="s">
+        <v>5</v>
+      </c>
+      <c r="G34" t="s">
+        <v>6</v>
+      </c>
+      <c r="H34" t="s">
+        <v>7</v>
+      </c>
+      <c r="I34" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>9</v>
+      </c>
+      <c r="B35">
+        <v>22595120</v>
+      </c>
+      <c r="C35">
+        <v>299</v>
+      </c>
+      <c r="D35" s="1">
+        <v>0.66400000000000003</v>
+      </c>
+      <c r="E35">
+        <v>2.54</v>
+      </c>
+      <c r="F35" s="1">
+        <v>0.11260000000000001</v>
+      </c>
+      <c r="G35" s="2">
+        <v>0</v>
+      </c>
+      <c r="H35" s="1">
+        <v>0.22120000000000001</v>
+      </c>
+      <c r="I35" s="1">
+        <v>4.0000000000000002E-4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>10</v>
+      </c>
+      <c r="B36">
+        <v>25589730</v>
+      </c>
+      <c r="C36">
+        <v>299</v>
+      </c>
+      <c r="D36" s="1">
+        <v>0.65980000000000005</v>
+      </c>
+      <c r="E36">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="F36" s="1">
+        <v>0.1027</v>
+      </c>
+      <c r="G36" s="2">
+        <v>0</v>
+      </c>
+      <c r="H36" s="1">
+        <v>0.23469999999999999</v>
+      </c>
+      <c r="I36" s="1">
+        <v>5.0000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>11</v>
+      </c>
+      <c r="B37">
+        <v>48528038</v>
+      </c>
+      <c r="C37">
+        <v>299</v>
+      </c>
+      <c r="D37" s="1">
+        <v>0.59060000000000001</v>
+      </c>
+      <c r="E37">
+        <v>2.2200000000000002</v>
+      </c>
+      <c r="F37" s="1">
+        <v>8.43E-2</v>
+      </c>
+      <c r="G37" s="2">
+        <v>0</v>
+      </c>
+      <c r="H37" s="1">
+        <v>0.3241</v>
+      </c>
+      <c r="I37" s="1">
+        <v>4.0000000000000002E-4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>12</v>
+      </c>
+      <c r="B38">
+        <v>41235603</v>
+      </c>
+      <c r="C38">
+        <v>299</v>
+      </c>
+      <c r="D38" s="2">
+        <v>0.63</v>
+      </c>
+      <c r="E38">
+        <v>2.23</v>
+      </c>
+      <c r="F38" s="1">
+        <v>0.11840000000000001</v>
+      </c>
+      <c r="G38" s="2">
+        <v>0</v>
+      </c>
+      <c r="H38" s="1">
+        <v>0.2505</v>
+      </c>
+      <c r="I38" s="1">
+        <v>5.9999999999999995E-4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>13</v>
+      </c>
+      <c r="B39">
+        <v>20852584</v>
+      </c>
+      <c r="C39">
+        <v>299</v>
+      </c>
+      <c r="D39" s="1">
+        <v>0.65280000000000005</v>
+      </c>
+      <c r="E39">
+        <v>2.37</v>
+      </c>
+      <c r="F39" s="1">
+        <v>0.1037</v>
+      </c>
+      <c r="G39" s="2">
+        <v>0</v>
+      </c>
+      <c r="H39" s="1">
+        <v>0.24229999999999999</v>
+      </c>
+      <c r="I39" s="1">
+        <v>5.0000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>14</v>
+      </c>
+      <c r="B40">
+        <v>18571158</v>
+      </c>
+      <c r="C40">
+        <v>299</v>
+      </c>
+      <c r="D40" s="1">
+        <v>0.67379999999999995</v>
+      </c>
+      <c r="E40">
+        <v>2.2200000000000002</v>
+      </c>
+      <c r="F40" s="1">
+        <v>0.1067</v>
+      </c>
+      <c r="G40" s="2">
+        <v>0</v>
+      </c>
+      <c r="H40" s="1">
+        <v>0.2185</v>
+      </c>
+      <c r="I40" s="1">
+        <v>2.9999999999999997E-4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>15</v>
+      </c>
+      <c r="B41">
+        <v>38680165</v>
+      </c>
+      <c r="C41">
+        <v>201</v>
+      </c>
+      <c r="D41" s="1">
+        <v>0.4143</v>
+      </c>
+      <c r="E41">
+        <v>2.57</v>
+      </c>
+      <c r="F41" s="1">
+        <v>7.3899999999999993E-2</v>
+      </c>
+      <c r="G41" s="2">
+        <v>0</v>
+      </c>
+      <c r="H41" s="1">
+        <v>0.51149999999999995</v>
+      </c>
+      <c r="I41" s="1">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>16</v>
+      </c>
+      <c r="B42">
+        <v>39743330</v>
+      </c>
+      <c r="C42">
+        <v>201</v>
+      </c>
+      <c r="D42" s="1">
+        <v>0.3987</v>
+      </c>
+      <c r="E42" s="4">
+        <v>2.52</v>
+      </c>
+      <c r="F42" s="1">
+        <v>7.3300000000000004E-2</v>
+      </c>
+      <c r="G42" s="2">
+        <v>0</v>
+      </c>
+      <c r="H42" s="1">
+        <v>0.52780000000000005</v>
+      </c>
+      <c r="I42" s="1">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>17</v>
+      </c>
+      <c r="B43">
+        <v>31208809</v>
+      </c>
+      <c r="C43">
+        <v>201</v>
+      </c>
+      <c r="D43" s="1">
+        <v>0.44409999999999999</v>
+      </c>
+      <c r="E43">
+        <v>2.48</v>
+      </c>
+      <c r="F43" s="1">
+        <v>7.8200000000000006E-2</v>
+      </c>
+      <c r="G43" s="2">
+        <v>0</v>
+      </c>
+      <c r="H43" s="1">
+        <v>0.47749999999999998</v>
+      </c>
+      <c r="I43" s="1">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>20</v>
+      </c>
+      <c r="B44">
+        <v>32802143</v>
+      </c>
+      <c r="C44">
+        <v>201</v>
+      </c>
+      <c r="D44" s="1">
+        <v>0.39850000000000002</v>
+      </c>
+      <c r="E44">
+        <v>2.63</v>
+      </c>
+      <c r="F44" s="1">
+        <v>7.4700000000000003E-2</v>
+      </c>
+      <c r="G44" s="2">
+        <v>0</v>
+      </c>
+      <c r="H44" s="1">
+        <v>0.52629999999999999</v>
+      </c>
+      <c r="I44" s="1">
+        <v>2.0000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>18</v>
+      </c>
+      <c r="B45">
+        <v>29613922</v>
+      </c>
+      <c r="C45">
+        <v>201</v>
+      </c>
+      <c r="D45" s="1">
+        <v>0.439</v>
+      </c>
+      <c r="E45">
+        <v>2.71</v>
+      </c>
+      <c r="F45" s="1">
+        <v>8.3299999999999999E-2</v>
+      </c>
+      <c r="G45" s="2">
+        <v>0</v>
+      </c>
+      <c r="H45" s="1">
+        <v>0.4773</v>
+      </c>
+      <c r="I45" s="1">
+        <v>2.0000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>19</v>
+      </c>
+      <c r="B46">
+        <v>35774916</v>
+      </c>
+      <c r="C46">
+        <v>201</v>
+      </c>
+      <c r="D46" s="1">
+        <v>0.45</v>
+      </c>
+      <c r="E46">
+        <v>2.75</v>
+      </c>
+      <c r="F46" s="1">
+        <v>8.3299999999999999E-2</v>
+      </c>
+      <c r="G46" s="2">
+        <v>0</v>
+      </c>
+      <c r="H46" s="1">
+        <v>0.46629999999999999</v>
+      </c>
+      <c r="I46" s="1">
+        <v>2.0000000000000001E-4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Testing with trimmomatic and HISAT2 for RNAseq alignment
</commit_message>
<xml_diff>
--- a/bioinformatics/Logs/RNAseq-alignment-stats.xlsx
+++ b/bioinformatics/Logs/RNAseq-alignment-stats.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bryce\Documents\scutellariaMetabolites\bioinformatics\Logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4989AAB9-EA61-4BCC-92EE-E0132EB850A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18516651-5C61-4821-9FF9-370220F820F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18570" yWindow="10755" windowWidth="19005" windowHeight="15600" activeTab="1" xr2:uid="{6382A5D9-1C64-42BE-963F-68A5DFDB5DBD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{6382A5D9-1C64-42BE-963F-68A5DFDB5DBD}"/>
   </bookViews>
   <sheets>
     <sheet name="STAR" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="30">
   <si>
     <t>Parameters set: --outFilterMismatchNmax 2</t>
   </si>
@@ -121,6 +121,9 @@
   </si>
   <si>
     <t>Overall alignment rate</t>
+  </si>
+  <si>
+    <t>With trimmomatic applied first to remove adapter sequences</t>
   </si>
 </sst>
 </file>
@@ -1667,10 +1670,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E156CE5-F208-4D86-9EB4-803CA7A75AFB}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1752,6 +1755,18 @@
       <c r="A7" t="s">
         <v>11</v>
       </c>
+      <c r="B7">
+        <v>38809128</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.91910000000000003</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.77690000000000003</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0.106</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -1904,6 +1919,93 @@
       </c>
       <c r="E16" s="1">
         <v>1.6E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rerunning bwa for SRR6940088 used PE option
</commit_message>
<xml_diff>
--- a/bioinformatics/Logs/RNAseq-alignment-stats.xlsx
+++ b/bioinformatics/Logs/RNAseq-alignment-stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bryce\Documents\scutellariaMetabolites\bioinformatics\Logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18516651-5C61-4821-9FF9-370220F820F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFA65A4D-A321-41AE-9C3E-F5291C7E3EA5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{6382A5D9-1C64-42BE-963F-68A5DFDB5DBD}"/>
+    <workbookView xWindow="1920" yWindow="600" windowWidth="19005" windowHeight="15600" activeTab="1" xr2:uid="{6382A5D9-1C64-42BE-963F-68A5DFDB5DBD}"/>
   </bookViews>
   <sheets>
     <sheet name="STAR" sheetId="1" r:id="rId1"/>
@@ -1673,7 +1673,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1952,60 +1952,204 @@
       <c r="A21" t="s">
         <v>9</v>
       </c>
+      <c r="B21">
+        <v>13505734</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0.88219999999999998</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0.71409999999999996</v>
+      </c>
+      <c r="E21" s="1">
+        <v>0.10340000000000001</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>10</v>
       </c>
+      <c r="B22">
+        <v>14027644</v>
+      </c>
+      <c r="C22" s="1">
+        <v>0.89580000000000004</v>
+      </c>
+      <c r="D22" s="1">
+        <v>0.73409999999999997</v>
+      </c>
+      <c r="E22" s="1">
+        <v>9.9099999999999994E-2</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>11</v>
       </c>
+      <c r="B23">
+        <v>36754327</v>
+      </c>
+      <c r="C23" s="1">
+        <v>0.69040000000000001</v>
+      </c>
+      <c r="D23" s="1">
+        <v>0.57989999999999997</v>
+      </c>
+      <c r="E23" s="1">
+        <v>7.4200000000000002E-2</v>
+      </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>12</v>
       </c>
+      <c r="B24">
+        <v>25753219</v>
+      </c>
+      <c r="C24" s="1">
+        <v>0.84530000000000005</v>
+      </c>
+      <c r="D24" s="1">
+        <v>0.68889999999999996</v>
+      </c>
+      <c r="E24" s="1">
+        <v>0.1043</v>
+      </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>13</v>
       </c>
+      <c r="B25">
+        <v>13000617</v>
+      </c>
+      <c r="C25" s="1">
+        <v>0.84570000000000001</v>
+      </c>
+      <c r="D25" s="2">
+        <v>70.260000000000005</v>
+      </c>
+      <c r="E25" s="1">
+        <v>8.9800000000000005E-2</v>
+      </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>14</v>
       </c>
+      <c r="B26">
+        <v>12337910</v>
+      </c>
+      <c r="C26" s="1">
+        <v>0.86160000000000003</v>
+      </c>
+      <c r="D26" s="1">
+        <v>0.72170000000000001</v>
+      </c>
+      <c r="E26" s="1">
+        <v>9.5000000000000001E-2</v>
+      </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>15</v>
       </c>
+      <c r="B27">
+        <v>38472891</v>
+      </c>
+      <c r="C27" s="1">
+        <v>0.19209999999999999</v>
+      </c>
+      <c r="D27" s="1">
+        <v>7.9600000000000004E-2</v>
+      </c>
+      <c r="E27" s="1">
+        <v>1.0699999999999999E-2</v>
+      </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>16</v>
       </c>
+      <c r="B28">
+        <v>39333015</v>
+      </c>
+      <c r="C28" s="1">
+        <v>0.19639999999999999</v>
+      </c>
+      <c r="D28" s="1">
+        <v>7.7200000000000005E-2</v>
+      </c>
+      <c r="E28" s="1">
+        <v>1.23E-2</v>
+      </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>17</v>
       </c>
+      <c r="B29">
+        <v>31005428</v>
+      </c>
+      <c r="C29" s="1">
+        <v>0.21510000000000001</v>
+      </c>
+      <c r="D29" s="1">
+        <v>8.4400000000000003E-2</v>
+      </c>
+      <c r="E29" s="1">
+        <v>1.17E-2</v>
+      </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>20</v>
       </c>
+      <c r="B30">
+        <v>32488347</v>
+      </c>
+      <c r="C30" s="1">
+        <v>0.18920000000000001</v>
+      </c>
+      <c r="D30" s="1">
+        <v>7.4700000000000003E-2</v>
+      </c>
+      <c r="E30" s="1">
+        <v>1.12E-2</v>
+      </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>18</v>
       </c>
+      <c r="B31">
+        <v>29327740</v>
+      </c>
+      <c r="C31" s="1">
+        <v>0.2094</v>
+      </c>
+      <c r="D31" s="1">
+        <v>8.5900000000000004E-2</v>
+      </c>
+      <c r="E31" s="1">
+        <v>1.4500000000000001E-2</v>
+      </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>19</v>
+      </c>
+      <c r="B32">
+        <v>35553788</v>
+      </c>
+      <c r="C32" s="1">
+        <v>0.2238</v>
+      </c>
+      <c r="D32" s="1">
+        <v>8.9499999999999996E-2</v>
+      </c>
+      <c r="E32" s="1">
+        <v>1.5900000000000001E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>